<commit_message>
changed frontend to netlify
</commit_message>
<xml_diff>
--- a/Yasine Burushaski/burushaski alphabets.xlsx
+++ b/Yasine Burushaski/burushaski alphabets.xlsx
@@ -706,10 +706,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -757,6 +757,81 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
@@ -765,16 +840,24 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -786,19 +869,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -810,21 +885,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -834,67 +894,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -917,187 +917,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1108,15 +1108,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1131,26 +1122,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1179,6 +1161,39 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1193,166 +1208,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1629,8 +1629,8 @@
   </sheetPr>
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>